<commit_message>
Updated firewall and role requirement Excel.
</commit_message>
<xml_diff>
--- a/Documentation/MHSA Data Analytics Platform - firewall and role requirement.xlsx
+++ b/Documentation/MHSA Data Analytics Platform - firewall and role requirement.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MHSA\Phase 2\Configurations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\mhsa\mhsa\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5341FE0-8CBE-425B-821E-EB558A329145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1CA167F-E056-4A0E-95D2-640F7440ED00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3024" yWindow="17172" windowWidth="23256" windowHeight="13176" xr2:uid="{0B31741D-4F11-412F-95C0-98021D53066D}"/>
+    <workbookView xWindow="3024" yWindow="17172" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{0B31741D-4F11-412F-95C0-98021D53066D}"/>
   </bookViews>
   <sheets>
     <sheet name="Firewall" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
   <si>
     <t xml:space="preserve">Source </t>
   </si>
@@ -184,6 +184,9 @@
   <si>
     <t>Azure DevOps Hostedagent  Agent
 ActiveMQ Message Processing</t>
+  </si>
+  <si>
+    <t>SYN_nonprod</t>
   </si>
 </sst>
 </file>
@@ -672,7 +675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D666D46-DCB5-4BB6-89B8-1CB8FBB2EF56}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A14"/>
     </sheetView>
   </sheetViews>
@@ -941,8 +944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AE1E493-45DE-4E77-A464-C4C2B2C0275B}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,7 +1030,7 @@
         <v>40</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>43</v>
@@ -1045,7 +1048,7 @@
         <v>41</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>44</v>

</xml_diff>